<commit_message>
Se corrige datos ejemplo
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00690C61-E094-4339-A4A3-C9FBAEB424AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179661B-49B0-4521-8E73-4B6FE2DCDE1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>ID</t>
   </si>
@@ -79,7 +79,10 @@
     <t>Itagüi</t>
   </si>
   <si>
-    <t>\# de telefono</t>
+    <t># de telefono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -924,7 +927,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,6 +942,9 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Se corrige nuevamente base de datos
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FF1194-810C-409B-9ECB-12BB257F50FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020C45F0-5888-413B-B63D-BA54DD386FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
-  <si>
-    <t>Ingreso</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>% pagado</t>
   </si>
@@ -70,9 +67,6 @@
     <t># de telefono</t>
   </si>
   <si>
-    <t>Posee-deuda-de-vivienda?</t>
-  </si>
-  <si>
     <t>$ID</t>
   </si>
   <si>
@@ -83,6 +77,12 @@
   </si>
   <si>
     <t>Costo vivienda?</t>
+  </si>
+  <si>
+    <t>Ingreso 1</t>
+  </si>
+  <si>
+    <t>Deuda-de-vivienda?</t>
   </si>
 </sst>
 </file>
@@ -934,28 +934,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>0</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -969,19 +969,19 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -995,16 +995,16 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>3114800</v>
       </c>
       <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
       </c>
       <c r="H3">
         <v>0.28999999999999998</v>
@@ -1021,13 +1021,13 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4">
         <v>3083500</v>
       </c>
       <c r="F4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G4">
         <v>405147000</v>
@@ -1047,13 +1047,13 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>630700</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>62708000</v>
@@ -1073,13 +1073,13 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <v>3114800</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G6">
         <v>728753400</v>
@@ -1099,19 +1099,19 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>3838000000</v>
       </c>
       <c r="H7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1125,13 +1125,13 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8">
         <v>3356600</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G8">
         <v>186855000</v>
@@ -1151,16 +1151,16 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9">
         <v>2204800</v>
       </c>
       <c r="F9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9">
         <v>0.05</v>
@@ -1177,19 +1177,16 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
         <v>3428900</v>
       </c>
       <c r="F10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G10">
         <v>539641705</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1203,10 +1200,10 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11">
         <v>169451000</v>

</xml_diff>

<commit_message>
Nuevos cambios en los nombres D:
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020C45F0-5888-413B-B63D-BA54DD386FF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C17D1-3A52-458E-AED6-24A672808ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,19 +70,19 @@
     <t>$ID</t>
   </si>
   <si>
-    <t>Estr@to</t>
-  </si>
-  <si>
     <t>MUNICIPIO</t>
   </si>
   <si>
-    <t>Costo vivienda?</t>
-  </si>
-  <si>
     <t>Ingreso 1</t>
   </si>
   <si>
     <t>Deuda-de-vivienda?</t>
+  </si>
+  <si>
+    <t>Costo_vivienda?</t>
+  </si>
+  <si>
+    <t>[Estrato]</t>
   </si>
 </sst>
 </file>
@@ -927,7 +927,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,19 +940,19 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" t="s">
-        <v>18</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Última modificación a base de datos (o eso espero)
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{652C17D1-3A52-458E-AED6-24A672808ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A1E37F-75AB-4251-8329-3E9D412890BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>% pagado</t>
   </si>
@@ -71,9 +71,6 @@
   </si>
   <si>
     <t>MUNICIPIO</t>
-  </si>
-  <si>
-    <t>Ingreso 1</t>
   </si>
   <si>
     <t>Deuda-de-vivienda?</t>
@@ -927,7 +924,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -940,19 +937,16 @@
         <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
       </c>
       <c r="H1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Ahora si, espero que sea la última ToT
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A1E37F-75AB-4251-8329-3E9D412890BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C46F3DD-71F8-4B1C-8CCE-8704EEE8C981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t>% pagado</t>
   </si>
@@ -80,6 +80,36 @@
   </si>
   <si>
     <t>[Estrato]</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>encuestado el 12 01 13</t>
+  </si>
+  <si>
+    <t>15 02 2013</t>
+  </si>
+  <si>
+    <t>encuestado el 15/12/15</t>
+  </si>
+  <si>
+    <t>6 Feb 13</t>
+  </si>
+  <si>
+    <t>15/02/2013</t>
+  </si>
+  <si>
+    <t>01/05/2013</t>
+  </si>
+  <si>
+    <t>7 Mar 14</t>
+  </si>
+  <si>
+    <t>23/09/2014</t>
+  </si>
+  <si>
+    <t>2/06/2014</t>
   </si>
 </sst>
 </file>
@@ -563,9 +593,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -921,288 +952,321 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
         <v>1035869</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>3126250</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>4</v>
       </c>
       <c r="H2" t="s">
         <v>4</v>
       </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
         <v>1035857</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>1192334</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>3114800</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
         <v>1007306</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>3434589</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>3083500</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>405147000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.31</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
         <v>3935563</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>7005931</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>630700</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>2</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>62708000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>0.18</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
         <v>1035857</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>1192334</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>3114800</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>6</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>728753400</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
         <v>2222985</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>8660538</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>9</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>3838000000</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
         <v>3488986</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>5625266</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>3356600</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>186855000</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
         <v>1022146</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>3979642</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>2204800</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
         <v>39359318</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>2304725</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>3428900</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>539641705</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
         <v>32321157</v>
       </c>
-      <c r="B11">
+      <c r="C11">
         <v>3952210</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>169451000</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>0.22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ahora si :D (creo)
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C46F3DD-71F8-4B1C-8CCE-8704EEE8C981}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566019A0-13E2-400E-A986-082AF81A21F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>% pagado</t>
   </si>
@@ -73,9 +73,6 @@
     <t>MUNICIPIO</t>
   </si>
   <si>
-    <t>Deuda-de-vivienda?</t>
-  </si>
-  <si>
     <t>Costo_vivienda?</t>
   </si>
   <si>
@@ -110,6 +107,15 @@
   </si>
   <si>
     <t>2/06/2014</t>
+  </si>
+  <si>
+    <t>Deuda-vivienda?</t>
+  </si>
+  <si>
+    <t>01 05 2013</t>
+  </si>
+  <si>
+    <t>municipio</t>
   </si>
 </sst>
 </file>
@@ -952,17 +958,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -971,24 +977,27 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
         <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2">
         <v>1035869</v>
@@ -1014,10 +1023,13 @@
       <c r="I2" t="s">
         <v>4</v>
       </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>1035857</v>
@@ -1043,10 +1055,13 @@
       <c r="I3">
         <v>0.28999999999999998</v>
       </c>
+      <c r="J3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4">
         <v>1007306</v>
@@ -1072,10 +1087,13 @@
       <c r="I4">
         <v>0.31</v>
       </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>3935563</v>
@@ -1101,10 +1119,13 @@
       <c r="I5">
         <v>0.18</v>
       </c>
+      <c r="J5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>1035857</v>
@@ -1130,10 +1151,13 @@
       <c r="I6">
         <v>0.28999999999999998</v>
       </c>
+      <c r="J6" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>2222985</v>
@@ -1159,10 +1183,13 @@
       <c r="I7" t="s">
         <v>2</v>
       </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>3488986</v>
@@ -1188,10 +1215,13 @@
       <c r="I8">
         <v>0.75</v>
       </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
         <v>1022146</v>
@@ -1217,10 +1247,13 @@
       <c r="I9">
         <v>0.05</v>
       </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10">
         <v>39359318</v>
@@ -1243,31 +1276,69 @@
       <c r="H10">
         <v>539641705</v>
       </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12">
         <v>32321157</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>3952210</v>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>6</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>169451000</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>0.22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se cambió un nombre ToT
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566019A0-13E2-400E-A986-082AF81A21F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D88633E-BDEE-42D1-9BA2-C7719D7866B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
     <t>01 05 2013</t>
   </si>
   <si>
-    <t>municipio</t>
+    <t>muni</t>
   </si>
 </sst>
 </file>
@@ -961,7 +961,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
se hace una corrección en una fila
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA6EBA4-B51A-48D7-AF47-6585AA07F1DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6284CF66-0D55-49DC-928D-0163D552929E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,7 +961,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>1035857</v>
@@ -1134,7 +1134,7 @@
         <v>1192334</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
         <v>5</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B7">
         <v>2222985</v>
@@ -1166,7 +1166,7 @@
         <v>8660538</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Otra corrección para el estrato D:
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6284CF66-0D55-49DC-928D-0163D552929E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46096AAC-A2BB-4687-B846-23E01B6FF681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,7 +961,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1102,7 +1102,7 @@
         <v>7005931</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Se modificó algo más D:
</commit_message>
<xml_diff>
--- a/Dataset/EjemploLimpieza.xlsx
+++ b/Dataset/EjemploLimpieza.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\jiperezga.github.io\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repo\pagina de control\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46096AAC-A2BB-4687-B846-23E01B6FF681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC660A13-F110-413F-B7BD-04DA622EF87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -961,7 +961,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>